<commit_message>
gammel modell med problemer ved constraints med indexhelvete
</commit_message>
<xml_diff>
--- a/Old Model/Input/model_input.xlsx
+++ b/Old Model/Input/model_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oyvindasplin/Documents/Indok/NTNU/Optimering/Master V22/master2022/Old Model/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5C61EA-2005-7249-971D-EA0BD98D0C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241984DA-359B-8745-B263-D3705C4C8FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19420" activeTab="3" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -11266,7 +11266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
   <dimension ref="A1:BX29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
@@ -22480,8 +22480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B305B3B2-E098-F04C-83CE-B18CE5C01F35}">
   <dimension ref="A1:AS32"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36924,21 +36924,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010014502AD36FC4D1459EE8BFEB917118AE" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b4cd19ef6f825a6ac181b2aef79b604">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1a062c2-eeb0-45d1-8c80-71eb2bb91349" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="944c6668d3530cb8510fee0a023b67da" ns2:_="">
     <xsd:import namespace="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
@@ -37110,31 +37095,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37150,4 +37126,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>